<commit_message>
Excel HR upload changes
</commit_message>
<xml_diff>
--- a/html/templates/ImportTrainingTemplate.xlsx
+++ b/html/templates/ImportTrainingTemplate.xlsx
@@ -76,15 +76,6 @@
     <t>Gender (Male/ Female)</t>
   </si>
   <si>
-    <t>Health Facility Name</t>
-  </si>
-  <si>
-    <t>LGA</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>Telephone number</t>
   </si>
   <si>
@@ -241,6 +232,78 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Cadre (e.g Nurse,Doctor,Midwife,CHO,CHEW)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Health Facility Name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> LGA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> State</t>
     </r>
   </si>
 </sst>
@@ -1015,7 +1078,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,13 +1114,13 @@
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="22" t="s">
@@ -1159,37 +1222,37 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="J17" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="K17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="L17" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="17" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1549,44 +1612,44 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>